<commit_message>
Corrected municipales election dates
</commit_message>
<xml_diff>
--- a/fondamentaux/data/results_by_districts_paris.xlsx
+++ b/fondamentaux/data/results_by_districts_paris.xlsx
@@ -527,7 +527,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>39591</v>
+        <v>39516</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -752,7 +752,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="n">
-        <v>41723</v>
+        <v>41721</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -1061,7 +1061,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="2" t="n">
-        <v>39591</v>
+        <v>39516</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -1286,7 +1286,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="2" t="n">
-        <v>41723</v>
+        <v>41721</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
@@ -1595,7 +1595,7 @@
         <v>26</v>
       </c>
       <c r="B28" s="2" t="n">
-        <v>39591</v>
+        <v>39516</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
@@ -1820,7 +1820,7 @@
         <v>31</v>
       </c>
       <c r="B33" s="2" t="n">
-        <v>41723</v>
+        <v>41721</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
@@ -2129,7 +2129,7 @@
         <v>38</v>
       </c>
       <c r="B40" s="2" t="n">
-        <v>39591</v>
+        <v>39516</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
@@ -2354,7 +2354,7 @@
         <v>43</v>
       </c>
       <c r="B45" s="2" t="n">
-        <v>41723</v>
+        <v>41721</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
@@ -2663,7 +2663,7 @@
         <v>50</v>
       </c>
       <c r="B52" s="2" t="n">
-        <v>39591</v>
+        <v>39516</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
@@ -2888,7 +2888,7 @@
         <v>55</v>
       </c>
       <c r="B57" s="2" t="n">
-        <v>41723</v>
+        <v>41721</v>
       </c>
       <c r="C57" t="inlineStr">
         <is>
@@ -3197,7 +3197,7 @@
         <v>62</v>
       </c>
       <c r="B64" s="2" t="n">
-        <v>39591</v>
+        <v>39516</v>
       </c>
       <c r="C64" t="inlineStr">
         <is>
@@ -3420,7 +3420,7 @@
         <v>67</v>
       </c>
       <c r="B69" s="2" t="n">
-        <v>41723</v>
+        <v>41721</v>
       </c>
       <c r="C69" t="inlineStr">
         <is>
@@ -3729,7 +3729,7 @@
         <v>74</v>
       </c>
       <c r="B76" s="2" t="n">
-        <v>39591</v>
+        <v>39516</v>
       </c>
       <c r="C76" t="inlineStr">
         <is>
@@ -3952,7 +3952,7 @@
         <v>79</v>
       </c>
       <c r="B81" s="2" t="n">
-        <v>41723</v>
+        <v>41721</v>
       </c>
       <c r="C81" t="inlineStr">
         <is>
@@ -4261,7 +4261,7 @@
         <v>86</v>
       </c>
       <c r="B88" s="2" t="n">
-        <v>39591</v>
+        <v>39516</v>
       </c>
       <c r="C88" t="inlineStr">
         <is>
@@ -4484,7 +4484,7 @@
         <v>91</v>
       </c>
       <c r="B93" s="2" t="n">
-        <v>41723</v>
+        <v>41721</v>
       </c>
       <c r="C93" t="inlineStr">
         <is>
@@ -4793,7 +4793,7 @@
         <v>98</v>
       </c>
       <c r="B100" s="2" t="n">
-        <v>39591</v>
+        <v>39516</v>
       </c>
       <c r="C100" t="inlineStr">
         <is>
@@ -5018,7 +5018,7 @@
         <v>103</v>
       </c>
       <c r="B105" s="2" t="n">
-        <v>41723</v>
+        <v>41721</v>
       </c>
       <c r="C105" t="inlineStr">
         <is>
@@ -5327,7 +5327,7 @@
         <v>110</v>
       </c>
       <c r="B112" s="2" t="n">
-        <v>39591</v>
+        <v>39516</v>
       </c>
       <c r="C112" t="inlineStr">
         <is>
@@ -5552,7 +5552,7 @@
         <v>115</v>
       </c>
       <c r="B117" s="2" t="n">
-        <v>41723</v>
+        <v>41721</v>
       </c>
       <c r="C117" t="inlineStr">
         <is>
@@ -5861,7 +5861,7 @@
         <v>122</v>
       </c>
       <c r="B124" s="2" t="n">
-        <v>39591</v>
+        <v>39516</v>
       </c>
       <c r="C124" t="inlineStr">
         <is>
@@ -6086,7 +6086,7 @@
         <v>127</v>
       </c>
       <c r="B129" s="2" t="n">
-        <v>41723</v>
+        <v>41721</v>
       </c>
       <c r="C129" t="inlineStr">
         <is>
@@ -6395,7 +6395,7 @@
         <v>134</v>
       </c>
       <c r="B136" s="2" t="n">
-        <v>39591</v>
+        <v>39516</v>
       </c>
       <c r="C136" t="inlineStr">
         <is>
@@ -6620,7 +6620,7 @@
         <v>139</v>
       </c>
       <c r="B141" s="2" t="n">
-        <v>41723</v>
+        <v>41721</v>
       </c>
       <c r="C141" t="inlineStr">
         <is>
@@ -6929,7 +6929,7 @@
         <v>146</v>
       </c>
       <c r="B148" s="2" t="n">
-        <v>39591</v>
+        <v>39516</v>
       </c>
       <c r="C148" t="inlineStr">
         <is>
@@ -7154,7 +7154,7 @@
         <v>151</v>
       </c>
       <c r="B153" s="2" t="n">
-        <v>41723</v>
+        <v>41721</v>
       </c>
       <c r="C153" t="inlineStr">
         <is>
@@ -7463,7 +7463,7 @@
         <v>158</v>
       </c>
       <c r="B160" s="2" t="n">
-        <v>39591</v>
+        <v>39516</v>
       </c>
       <c r="C160" t="inlineStr">
         <is>
@@ -7688,7 +7688,7 @@
         <v>163</v>
       </c>
       <c r="B165" s="2" t="n">
-        <v>41723</v>
+        <v>41721</v>
       </c>
       <c r="C165" t="inlineStr">
         <is>
@@ -7997,7 +7997,7 @@
         <v>170</v>
       </c>
       <c r="B172" s="2" t="n">
-        <v>39591</v>
+        <v>39516</v>
       </c>
       <c r="C172" t="inlineStr">
         <is>
@@ -8222,7 +8222,7 @@
         <v>175</v>
       </c>
       <c r="B177" s="2" t="n">
-        <v>41723</v>
+        <v>41721</v>
       </c>
       <c r="C177" t="inlineStr">
         <is>
@@ -8531,7 +8531,7 @@
         <v>182</v>
       </c>
       <c r="B184" s="2" t="n">
-        <v>39591</v>
+        <v>39516</v>
       </c>
       <c r="C184" t="inlineStr">
         <is>
@@ -8754,7 +8754,7 @@
         <v>187</v>
       </c>
       <c r="B189" s="2" t="n">
-        <v>41723</v>
+        <v>41721</v>
       </c>
       <c r="C189" t="inlineStr">
         <is>
@@ -9063,7 +9063,7 @@
         <v>194</v>
       </c>
       <c r="B196" s="2" t="n">
-        <v>39591</v>
+        <v>39516</v>
       </c>
       <c r="C196" t="inlineStr">
         <is>
@@ -9288,7 +9288,7 @@
         <v>199</v>
       </c>
       <c r="B201" s="2" t="n">
-        <v>41723</v>
+        <v>41721</v>
       </c>
       <c r="C201" t="inlineStr">
         <is>
@@ -9597,7 +9597,7 @@
         <v>206</v>
       </c>
       <c r="B208" s="2" t="n">
-        <v>39591</v>
+        <v>39516</v>
       </c>
       <c r="C208" t="inlineStr">
         <is>
@@ -9822,7 +9822,7 @@
         <v>211</v>
       </c>
       <c r="B213" s="2" t="n">
-        <v>41723</v>
+        <v>41721</v>
       </c>
       <c r="C213" t="inlineStr">
         <is>
@@ -10131,7 +10131,7 @@
         <v>218</v>
       </c>
       <c r="B220" s="2" t="n">
-        <v>39591</v>
+        <v>39516</v>
       </c>
       <c r="C220" t="inlineStr">
         <is>
@@ -10356,7 +10356,7 @@
         <v>223</v>
       </c>
       <c r="B225" s="2" t="n">
-        <v>41723</v>
+        <v>41721</v>
       </c>
       <c r="C225" t="inlineStr">
         <is>
@@ -10665,7 +10665,7 @@
         <v>230</v>
       </c>
       <c r="B232" s="2" t="n">
-        <v>39591</v>
+        <v>39516</v>
       </c>
       <c r="C232" t="inlineStr">
         <is>
@@ -10890,7 +10890,7 @@
         <v>235</v>
       </c>
       <c r="B237" s="2" t="n">
-        <v>41723</v>
+        <v>41721</v>
       </c>
       <c r="C237" t="inlineStr">
         <is>

</xml_diff>